<commit_message>
reviewed with class, made notes and changed absolute references
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a90fe9adf95d6e93/Desktop/NSS - Data Analytics 9/Excel/lookups_exercise-mjbeall09876/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0879AB71-01C6-4024-964A-C246DFBB00F6}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12A5F847-23F1-4567-B6B8-233A8182834C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -914,7 +914,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Arts Commission Budget and Actual</a:t>
+              <a:t>Budget and Actual</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1872,6 +1872,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2171,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2254,8 +2258,8 @@
         <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
-        <f>IFERROR(D2/C2, "0")</f>
-        <v>-4.5118552552396413E-2</v>
+        <f>IFERROR(D2/B2, "0")</f>
+        <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
         <f>_xlfn.RANK.EQ(E2,$E$2:$E$52,1)</f>
@@ -2313,8 +2317,8 @@
         <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E52" si="1">IFERROR(D3/C3, "0")</f>
-        <v>-2.3614774160787572E-2</v>
+        <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3, "0")</f>
+        <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F52" si="2">_xlfn.RANK.EQ(E3,$E$2:$E$52,1)</f>
@@ -2373,7 +2377,7 @@
       </c>
       <c r="E4" s="5">
         <f t="shared" si="1"/>
-        <v>-4.9571938826780369E-3</v>
+        <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
@@ -2432,7 +2436,7 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>-0.10408662796074925</v>
+        <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
@@ -2491,7 +2495,7 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>-6.0614054335986108E-2</v>
+        <v>-5.7149963352064452E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
@@ -2550,7 +2554,7 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" si="1"/>
-        <v>-0.12997947527548054</v>
+        <v>-0.11502817362571344</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
@@ -2609,7 +2613,7 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" si="1"/>
-        <v>-0.17974498338738901</v>
+        <v>-0.15235918433091292</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
@@ -2668,7 +2672,7 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" si="1"/>
-        <v>-4.4296041483789649E-2</v>
+        <v>-4.2417130511048909E-2</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
@@ -2727,7 +2731,7 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" si="1"/>
-        <v>-8.8947400057633408E-2</v>
+        <v>-8.1681998646514792E-2</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
@@ -2845,7 +2849,7 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" si="1"/>
-        <v>-5.2698794104010328E-2</v>
+        <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
@@ -2904,7 +2908,7 @@
       </c>
       <c r="E13" s="5">
         <f t="shared" si="1"/>
-        <v>-1.308175643402067E-2</v>
+        <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
@@ -2963,7 +2967,7 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" si="1"/>
-        <v>-1.3826514521668838E-2</v>
+        <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
@@ -3022,7 +3026,7 @@
       </c>
       <c r="E15" s="5">
         <f t="shared" si="1"/>
-        <v>3.173636849285945E-3</v>
+        <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
@@ -3081,7 +3085,7 @@
       </c>
       <c r="E16" s="5">
         <f t="shared" si="1"/>
-        <v>-1.1992299628906885E-2</v>
+        <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
@@ -3140,7 +3144,7 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" si="1"/>
-        <v>-2.9178332498198175E-2</v>
+        <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
@@ -3199,7 +3203,7 @@
       </c>
       <c r="E18" s="5">
         <f t="shared" si="1"/>
-        <v>-5.7123801176609125E-2</v>
+        <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
@@ -3258,7 +3262,7 @@
       </c>
       <c r="E19" s="5">
         <f t="shared" si="1"/>
-        <v>-4.4479191210760792E-2</v>
+        <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
@@ -3317,7 +3321,7 @@
       </c>
       <c r="E20" s="5">
         <f t="shared" si="1"/>
-        <v>-1.237969145816416E-5</v>
+        <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
@@ -3376,7 +3380,7 @@
       </c>
       <c r="E21" s="5">
         <f t="shared" si="1"/>
-        <v>-8.5838183495867346E-2</v>
+        <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
@@ -3435,7 +3439,7 @@
       </c>
       <c r="E22" s="5">
         <f t="shared" si="1"/>
-        <v>-1.3464383431954106E-2</v>
+        <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
@@ -3494,7 +3498,7 @@
       </c>
       <c r="E23" s="5">
         <f t="shared" si="1"/>
-        <v>-4.1222097478569475E-2</v>
+        <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
@@ -3553,7 +3557,7 @@
       </c>
       <c r="E24" s="5">
         <f t="shared" si="1"/>
-        <v>-1.3515167295364007E-2</v>
+        <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
@@ -3612,7 +3616,7 @@
       </c>
       <c r="E25" s="5">
         <f t="shared" si="1"/>
-        <v>-1.0331785152747561E-2</v>
+        <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
@@ -3671,7 +3675,7 @@
       </c>
       <c r="E26" s="5">
         <f t="shared" si="1"/>
-        <v>-9.3261899836535073E-2</v>
+        <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
@@ -3789,7 +3793,7 @@
       </c>
       <c r="E28" s="5">
         <f t="shared" si="1"/>
-        <v>-0.10592892583696122</v>
+        <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
@@ -3848,7 +3852,7 @@
       </c>
       <c r="E29" s="5">
         <f t="shared" si="1"/>
-        <v>-1.5022591899611784E-2</v>
+        <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
@@ -3907,7 +3911,7 @@
       </c>
       <c r="E30" s="5">
         <f t="shared" si="1"/>
-        <v>-8.454008551485875E-3</v>
+        <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
@@ -3966,7 +3970,7 @@
       </c>
       <c r="E31" s="5">
         <f t="shared" si="1"/>
-        <v>-1.4230190697391801E-2</v>
+        <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
@@ -4025,7 +4029,7 @@
       </c>
       <c r="E32" s="5">
         <f t="shared" si="1"/>
-        <v>-1.2447990154890821E-2</v>
+        <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
@@ -4084,7 +4088,7 @@
       </c>
       <c r="E33" s="5">
         <f t="shared" si="1"/>
-        <v>-8.0614605229348581E-3</v>
+        <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
@@ -4143,7 +4147,7 @@
       </c>
       <c r="E34" s="5">
         <f t="shared" si="1"/>
-        <v>-1.9304765584697302E-2</v>
+        <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
@@ -4261,7 +4265,7 @@
       </c>
       <c r="E36" s="5">
         <f t="shared" si="1"/>
-        <v>-8.5361344557927391E-2</v>
+        <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
@@ -4320,7 +4324,7 @@
       </c>
       <c r="E37" s="5">
         <f t="shared" si="1"/>
-        <v>-4.1064276249856521E-2</v>
+        <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
@@ -4379,7 +4383,7 @@
       </c>
       <c r="E38" s="5">
         <f t="shared" si="1"/>
-        <v>-1.9829233869414847E-2</v>
+        <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
@@ -4438,7 +4442,7 @@
       </c>
       <c r="E39" s="5">
         <f t="shared" si="1"/>
-        <v>-8.7062302001452777E-2</v>
+        <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
@@ -4497,7 +4501,7 @@
       </c>
       <c r="E40" s="5">
         <f t="shared" si="1"/>
-        <v>-2.1742447906733384E-2</v>
+        <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
@@ -4556,7 +4560,7 @@
       </c>
       <c r="E41" s="5">
         <f t="shared" si="1"/>
-        <v>-4.1786635070699275E-2</v>
+        <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
@@ -4615,7 +4619,7 @@
       </c>
       <c r="E42" s="5">
         <f t="shared" si="1"/>
-        <v>-2.207581547652165E-4</v>
+        <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
@@ -4674,7 +4678,7 @@
       </c>
       <c r="E43" s="5">
         <f t="shared" si="1"/>
-        <v>-2.0926287045185434E-2</v>
+        <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
@@ -4733,7 +4737,7 @@
       </c>
       <c r="E44" s="5">
         <f t="shared" si="1"/>
-        <v>-9.8725902010485707E-3</v>
+        <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
@@ -4792,7 +4796,7 @@
       </c>
       <c r="E45" s="5">
         <f t="shared" si="1"/>
-        <v>-1.3043073369966466E-2</v>
+        <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
@@ -4851,7 +4855,7 @@
       </c>
       <c r="E46" s="5">
         <f t="shared" si="1"/>
-        <v>-3.0100754316998604E-3</v>
+        <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
@@ -4910,7 +4914,7 @@
       </c>
       <c r="E47" s="5">
         <f t="shared" si="1"/>
-        <v>-1.7438980340993323E-4</v>
+        <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
@@ -4969,7 +4973,7 @@
       </c>
       <c r="E48" s="5">
         <f t="shared" si="1"/>
-        <v>-3.2133614317697297E-2</v>
+        <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
@@ -5028,7 +5032,7 @@
       </c>
       <c r="E49" s="5">
         <f t="shared" si="1"/>
-        <v>-1.8790947081103241E-2</v>
+        <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
@@ -5146,7 +5150,7 @@
       </c>
       <c r="E51" s="5">
         <f t="shared" si="1"/>
-        <v>-1.295083556790318E-2</v>
+        <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
@@ -5205,7 +5209,7 @@
       </c>
       <c r="E52" s="5">
         <f t="shared" si="1"/>
-        <v>-8.706990884047304E-2</v>
+        <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
@@ -5276,11 +5280,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56,A2:I53,9,FALSE)</f>
+        <f>VLOOKUP(A56,$A$2:$I$53,9,FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f>VLOOKUP(A56,A2:P52,14,FALSE)</f>
+        <f>VLOOKUP(A56,$A$2:$P$52,14,FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5293,11 +5297,11 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="10">VLOOKUP(A57,A3:I54,9,FALSE)</f>
+        <f t="shared" ref="C57:C61" si="10">VLOOKUP(A57,$A$2:$I$53,9,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57,A3:P53,14,FALSE)</f>
+        <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57,$A$2:$P$52,14,FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5514,15 +5518,15 @@
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX(D2:D52,MATCH(A74,A2:A52))</f>
+        <f>INDEX($D$2:$D$52,MATCH($A74,$A$2:$A$52))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f>INDEX(I2:I52,MATCH(A74,A2:A52))</f>
+        <f>INDEX($I$2:$I$52,MATCH($A74,$A$2:$A$52))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f>INDEX(N2:N52,MATCH(A74,A2:A52))</f>
+        <f>INDEX($N$2:$N$52,MATCH($A74,$A$2:$A$52))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5531,15 +5535,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="15">INDEX(D3:D53,MATCH(A75,A3:A53))</f>
+        <f t="shared" ref="B75:B79" si="15">INDEX($D$2:$D$52,MATCH($A75,$A$2:$A$52))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="16">INDEX(I3:I53,MATCH(A75,A3:A53))</f>
+        <f t="shared" ref="C75:C79" si="16">INDEX($I$2:$I$52,MATCH($A75,$A$2:$A$52))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="17">INDEX(N3:N53,MATCH(A75,A3:A53))</f>
+        <f t="shared" ref="D75:D79" si="17">INDEX($N$2:$N$52,MATCH($A75,$A$2:$A$52))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>

</xml_diff>